<commit_message>
Last update of simulation results
- in future this should be in the gitignore list!
</commit_message>
<xml_diff>
--- a/simulation_results/test/inputs/input_template_excel.xlsx
+++ b/simulation_results/test/inputs/input_template_excel.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="283">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -2978,7 +2978,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
@@ -3120,20 +3120,6 @@
       </c>
       <c r="D11" s="20" t="n">
         <v>100</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="B12" s="20" t="n">
-        <v>15</v>
-      </c>
-      <c r="C12" s="20" t="n">
-        <v>25</v>
-      </c>
-      <c r="D12" s="20" t="n">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -16643,8 +16629,8 @@
   </sheetPr>
   <dimension ref="A1:AMD36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -32033,10 +32019,10 @@
         <v>39</v>
       </c>
       <c r="C17" s="39" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D17" s="39" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E17" s="39" t="s">
         <v>41</v>
@@ -32060,7 +32046,7 @@
         <v>41</v>
       </c>
       <c r="E18" s="39" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="AMA18" s="0"/>
       <c r="AMB18" s="0"/>

</xml_diff>

<commit_message>
Testing the fuel price function (unfinished)
</commit_message>
<xml_diff>
--- a/simulation_results/test/inputs/input_template_excel.xlsx
+++ b/simulation_results/test/inputs/input_template_excel.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="283">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -2978,7 +2978,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
@@ -3120,6 +3120,20 @@
       </c>
       <c r="D11" s="20" t="n">
         <v>100</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B12" s="20" t="n">
+        <v>15</v>
+      </c>
+      <c r="C12" s="20" t="n">
+        <v>25</v>
+      </c>
+      <c r="D12" s="20" t="n">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -16629,8 +16643,8 @@
   </sheetPr>
   <dimension ref="A1:AMD36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -32019,10 +32033,10 @@
         <v>39</v>
       </c>
       <c r="C17" s="39" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D17" s="39" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E17" s="39" t="s">
         <v>41</v>
@@ -32046,7 +32060,7 @@
         <v>41</v>
       </c>
       <c r="E18" s="39" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="AMA18" s="0"/>
       <c r="AMB18" s="0"/>

</xml_diff>

<commit_message>
Remove unnecessary try/except and a comma.
</commit_message>
<xml_diff>
--- a/simulation_results/test/inputs/input_template_excel.xlsx
+++ b/simulation_results/test/inputs/input_template_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="345">
   <si>
     <t xml:space="preserve">Tool for optimizing and simulating off- and on-grid electrification solutions</t>
   </si>
@@ -1340,7 +1340,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="70">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1589,19 +1589,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1918,13 +1910,13 @@
   </sheetPr>
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="18.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.54"/>
@@ -2374,7 +2366,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="6.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="24" width="6.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="24" width="6.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="4" style="0" width="8.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="6.09"/>
   </cols>
@@ -3423,12 +3415,12 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="20" width="12.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="20" width="12.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="9.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="20" width="6.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="8.54"/>
@@ -3552,26 +3544,13 @@
         <v>1000</v>
       </c>
       <c r="C11" s="20" t="n">
-        <v>1200</v>
+        <v>1100</v>
       </c>
       <c r="D11" s="20" t="n">
         <v>100</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="20" t="s">
-        <v>159</v>
-      </c>
-      <c r="B12" s="20" t="n">
-        <v>15</v>
-      </c>
-      <c r="C12" s="20" t="n">
-        <v>25</v>
-      </c>
-      <c r="D12" s="20" t="n">
-        <v>5</v>
-      </c>
-    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="B3:G3"/>
@@ -3612,8 +3591,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="20" width="8.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="20" width="9.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="10" style="20" width="6.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="20" width="12.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="20" width="11.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="20" width="12.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="20" width="11.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="21" style="20" width="6.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="6.91"/>
   </cols>
@@ -4413,15 +4392,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N36"/>
+  <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B43" activeCellId="0" sqref="B43"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.54"/>
@@ -4667,10 +4646,10 @@
       <c r="B21" s="61" t="s">
         <v>321</v>
       </c>
-      <c r="C21" s="62" t="s">
+      <c r="C21" s="47" t="s">
         <v>322</v>
       </c>
-      <c r="D21" s="63" t="n">
+      <c r="D21" s="62" t="n">
         <v>0.238492063492063</v>
       </c>
       <c r="E21" s="56"/>
@@ -4686,22 +4665,22 @@
       <c r="B22" s="61" t="s">
         <v>323</v>
       </c>
-      <c r="C22" s="62" t="s">
+      <c r="C22" s="47" t="s">
         <v>324</v>
       </c>
-      <c r="D22" s="63" t="n">
+      <c r="D22" s="62" t="n">
         <v>0.246825396825397</v>
       </c>
-      <c r="E22" s="64" t="n">
+      <c r="E22" s="63" t="n">
         <v>2.75</v>
       </c>
-      <c r="F22" s="65" t="s">
+      <c r="F22" s="57" t="s">
         <v>187</v>
       </c>
-      <c r="G22" s="65" t="n">
+      <c r="G22" s="57" t="n">
         <v>1.88</v>
       </c>
-      <c r="H22" s="65" t="n">
+      <c r="H22" s="57" t="n">
         <v>3</v>
       </c>
       <c r="I22" s="57" t="s">
@@ -4719,16 +4698,16 @@
       <c r="D23" s="60" t="n">
         <v>0.254811507936508</v>
       </c>
-      <c r="E23" s="64" t="n">
+      <c r="E23" s="63" t="n">
         <v>2.25</v>
       </c>
-      <c r="F23" s="65" t="s">
+      <c r="F23" s="57" t="s">
         <v>187</v>
       </c>
-      <c r="G23" s="65" t="n">
+      <c r="G23" s="57" t="n">
         <v>1.5</v>
       </c>
-      <c r="H23" s="65" t="n">
+      <c r="H23" s="57" t="n">
         <v>3</v>
       </c>
       <c r="I23" s="57" t="s">
@@ -4736,44 +4715,44 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="66" t="s">
+      <c r="A24" s="64" t="s">
         <v>327</v>
       </c>
-      <c r="B24" s="67" t="s">
+      <c r="B24" s="65" t="s">
         <v>328</v>
       </c>
-      <c r="C24" s="62" t="s">
+      <c r="C24" s="47" t="s">
         <v>329</v>
       </c>
-      <c r="D24" s="63" t="n">
+      <c r="D24" s="62" t="n">
         <v>0.265354437229437</v>
       </c>
-      <c r="E24" s="64" t="n">
+      <c r="E24" s="63" t="n">
         <v>2</v>
       </c>
-      <c r="F24" s="65" t="s">
+      <c r="F24" s="57" t="s">
         <v>187</v>
       </c>
-      <c r="G24" s="65" t="n">
+      <c r="G24" s="57" t="n">
         <v>2.6</v>
       </c>
-      <c r="H24" s="65" t="n">
+      <c r="H24" s="57" t="n">
         <v>2.17</v>
       </c>
       <c r="I24" s="57" t="s">
         <v>330</v>
       </c>
-      <c r="N24" s="68"/>
+      <c r="N24" s="66"/>
     </row>
     <row r="25" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="66"/>
-      <c r="B25" s="67" t="s">
+      <c r="A25" s="64"/>
+      <c r="B25" s="65" t="s">
         <v>331</v>
       </c>
-      <c r="C25" s="62" t="s">
+      <c r="C25" s="47" t="s">
         <v>332</v>
       </c>
-      <c r="D25" s="63" t="n">
+      <c r="D25" s="62" t="n">
         <v>0.3964420995671</v>
       </c>
       <c r="E25" s="56"/>
@@ -4783,11 +4762,11 @@
       <c r="I25" s="57" t="s">
         <v>315</v>
       </c>
-      <c r="N25" s="68"/>
+      <c r="N25" s="66"/>
     </row>
     <row r="26" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="66"/>
-      <c r="B26" s="69" t="s">
+      <c r="A26" s="64"/>
+      <c r="B26" s="67" t="s">
         <v>333</v>
       </c>
       <c r="C26" s="59" t="s">
@@ -4796,28 +4775,28 @@
       <c r="D26" s="60" t="n">
         <v>0.338203463203463</v>
       </c>
-      <c r="E26" s="64" t="n">
+      <c r="E26" s="63" t="n">
         <v>2.57</v>
       </c>
-      <c r="F26" s="65" t="s">
+      <c r="F26" s="57" t="s">
         <v>187</v>
       </c>
-      <c r="G26" s="65" t="n">
+      <c r="G26" s="57" t="n">
         <v>1.71</v>
       </c>
-      <c r="H26" s="65" t="n">
+      <c r="H26" s="57" t="n">
         <v>2.14</v>
       </c>
       <c r="I26" s="57" t="s">
         <v>330</v>
       </c>
-      <c r="N26" s="68"/>
+      <c r="N26" s="66"/>
     </row>
     <row r="27" customFormat="false" ht="12.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="70" t="s">
+      <c r="A27" s="68" t="s">
         <v>335</v>
       </c>
-      <c r="B27" s="71" t="s">
+      <c r="B27" s="69" t="s">
         <v>336</v>
       </c>
       <c r="C27" s="54" t="s">
@@ -4826,16 +4805,16 @@
       <c r="D27" s="55" t="n">
         <v>0.255808080808081</v>
       </c>
-      <c r="E27" s="64" t="n">
+      <c r="E27" s="63" t="n">
         <v>0</v>
       </c>
-      <c r="F27" s="65" t="s">
+      <c r="F27" s="57" t="s">
         <v>187</v>
       </c>
-      <c r="G27" s="65" t="n">
+      <c r="G27" s="57" t="n">
         <v>0.77</v>
       </c>
-      <c r="H27" s="65" t="n">
+      <c r="H27" s="57" t="n">
         <v>0.44</v>
       </c>
       <c r="I27" s="57" t="s">
@@ -4846,26 +4825,26 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="70"/>
-      <c r="B28" s="67" t="s">
+      <c r="A28" s="68"/>
+      <c r="B28" s="65" t="s">
         <v>339</v>
       </c>
-      <c r="C28" s="62" t="s">
+      <c r="C28" s="47" t="s">
         <v>340</v>
       </c>
-      <c r="D28" s="63" t="n">
+      <c r="D28" s="62" t="n">
         <v>0.383775252525253</v>
       </c>
-      <c r="E28" s="64" t="n">
+      <c r="E28" s="63" t="n">
         <v>2.63</v>
       </c>
-      <c r="F28" s="65" t="s">
+      <c r="F28" s="57" t="s">
         <v>187</v>
       </c>
-      <c r="G28" s="65" t="n">
+      <c r="G28" s="57" t="n">
         <v>1</v>
       </c>
-      <c r="H28" s="65" t="n">
+      <c r="H28" s="57" t="n">
         <v>1.88</v>
       </c>
       <c r="I28" s="57" t="s">
@@ -4873,8 +4852,8 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="70"/>
-      <c r="B29" s="69" t="s">
+      <c r="A29" s="68"/>
+      <c r="B29" s="67" t="s">
         <v>341</v>
       </c>
       <c r="C29" s="59" t="s">
@@ -4883,16 +4862,16 @@
       <c r="D29" s="60" t="n">
         <v>0.360416666666667</v>
       </c>
-      <c r="E29" s="64" t="n">
+      <c r="E29" s="63" t="n">
         <v>1.63</v>
       </c>
-      <c r="F29" s="65" t="s">
+      <c r="F29" s="57" t="s">
         <v>187</v>
       </c>
-      <c r="G29" s="65" t="n">
+      <c r="G29" s="57" t="n">
         <v>1.5</v>
       </c>
-      <c r="H29" s="65" t="n">
+      <c r="H29" s="57" t="n">
         <v>2.63</v>
       </c>
       <c r="I29" s="57" t="s">
@@ -4930,16 +4909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="47" t="str">
-        <f aca="false">IF(input_sensitivity!A12 = "","",input_sensitivity!A12)</f>
-        <v>pv_lifetime</v>
-      </c>
-      <c r="B35" s="47" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>